<commit_message>
excel sheet that helps with which solumns to keep and which to remove in order to help create an OLAP database for Power BI
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://reliablecollaboration-my.sharepoint.com/personal/bess_rcc_team/Documents/Courseware/DataAnalyticsWeek5-8/Student Files/Week 9 downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA878EF4-4B80-439A-88BC-05CECC90D1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F833DE9-886A-4AEF-903D-981C8A99B556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Northwind Columns" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="95">
   <si>
     <t>table_name</t>
   </si>
@@ -308,6 +308,18 @@
   </si>
   <si>
     <t>New Name?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>varchar</t>
   </si>
 </sst>
 </file>
@@ -695,27 +707,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B56A5E-AA28-4DB9-BAE3-51DE131C631E}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B75" sqref="A75:XFD75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" customWidth="1"/>
-    <col min="2" max="2" width="10.265625" customWidth="1"/>
-    <col min="3" max="3" width="17.1328125" customWidth="1"/>
-    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.265625" customWidth="1"/>
-    <col min="7" max="7" width="17.86328125" customWidth="1"/>
-    <col min="9" max="9" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.59765625" customWidth="1"/>
-    <col min="13" max="13" width="11.59765625" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,7 +772,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -775,8 +788,17 @@
       <c r="E2" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -792,8 +814,14 @@
       <c r="E3" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -809,8 +837,11 @@
       <c r="E4" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="K4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -826,8 +857,11 @@
       <c r="E5" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="K5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -843,8 +877,14 @@
       <c r="E6" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -860,8 +900,14 @@
       <c r="E7" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J7" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -877,8 +923,11 @@
       <c r="E8" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="L8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -894,8 +943,11 @@
       <c r="E9" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="L9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -912,7 +964,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -928,8 +980,11 @@
       <c r="E11" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="K11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -946,7 +1001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -963,7 +1018,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -980,7 +1035,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -996,8 +1051,11 @@
       <c r="E15" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="K15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1013,8 +1071,11 @@
       <c r="E16" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1030,8 +1091,14 @@
       <c r="E17" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1048,7 +1115,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1065,7 +1132,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
@@ -1082,7 +1149,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1099,7 +1166,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1116,7 +1183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1133,7 +1200,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1149,8 +1216,11 @@
       <c r="E24" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1167,7 +1237,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1184,7 +1254,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1201,7 +1271,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1218,7 +1288,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1234,8 +1304,11 @@
       <c r="E29" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1251,8 +1324,11 @@
       <c r="E30" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1268,8 +1344,11 @@
       <c r="E31" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1285,8 +1364,11 @@
       <c r="E32" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -1303,7 +1385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -1319,8 +1401,11 @@
       <c r="E34" s="1">
         <v>510</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
@@ -1336,8 +1421,14 @@
       <c r="E35" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
@@ -1353,8 +1444,14 @@
       <c r="E36" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G36" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
@@ -1370,8 +1467,14 @@
       <c r="E37" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1388,7 +1491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1405,7 +1508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1422,7 +1525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1439,7 +1542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -1455,8 +1558,14 @@
       <c r="E42" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
@@ -1472,8 +1581,14 @@
       <c r="E43" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G43" t="s">
+        <v>91</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -1489,8 +1604,14 @@
       <c r="E44" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G44" t="s">
+        <v>91</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>53</v>
       </c>
@@ -1506,8 +1627,11 @@
       <c r="E45" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H45" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -1524,7 +1648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
@@ -1540,8 +1664,11 @@
       <c r="E47" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H47" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -1558,7 +1685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -1575,7 +1702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
@@ -1591,8 +1718,11 @@
       <c r="E50" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="I50" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
@@ -1609,7 +1739,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
@@ -1626,7 +1756,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>53</v>
       </c>
@@ -1643,7 +1773,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -1660,7 +1790,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -1677,7 +1807,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1693,8 +1823,14 @@
       <c r="E56" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -1710,8 +1846,11 @@
       <c r="E57" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="I57" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1727,8 +1866,14 @@
       <c r="E58" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G58" t="s">
+        <v>91</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
@@ -1744,8 +1889,14 @@
       <c r="E59" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G59" t="s">
+        <v>91</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -1762,7 +1913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
@@ -1779,7 +1930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
@@ -1796,7 +1947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
@@ -1813,7 +1964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
@@ -1830,7 +1981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
@@ -1847,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>22</v>
       </c>
@@ -1863,8 +2014,14 @@
       <c r="E66" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>22</v>
       </c>
@@ -1881,7 +2038,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>76</v>
       </c>
@@ -1898,7 +2055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>76</v>
       </c>
@@ -1915,7 +2072,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
@@ -1932,7 +2089,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>78</v>
       </c>
@@ -1948,8 +2105,14 @@
       <c r="E71" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F71" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>78</v>
       </c>
@@ -1965,8 +2128,11 @@
       <c r="E72" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="I72" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -1983,7 +2149,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
@@ -2000,7 +2166,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>78</v>
       </c>
@@ -2016,8 +2182,11 @@
       <c r="E75" s="2">
         <v>120</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K75" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -2034,7 +2203,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
@@ -2051,7 +2220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
@@ -2068,7 +2237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -2085,7 +2254,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
@@ -2101,8 +2270,11 @@
       <c r="E80" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K80" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>78</v>
       </c>
@@ -2118,8 +2290,11 @@
       <c r="E81" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K81" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>78</v>
       </c>
@@ -2136,7 +2311,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -2152,8 +2327,14 @@
       <c r="E83" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>80</v>
       </c>
@@ -2170,7 +2351,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>80</v>
       </c>
@@ -2185,6 +2366,15 @@
       </c>
       <c r="E85" s="1">
         <v>4</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K85" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2202,6 +2392,25 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA5D0A6329BB324E86983B32928CFC2E" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b28f3bc5995c0091f528145aa367664">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xmlns:ns3="ced60a7f-99b1-48d2-b555-34851c8026ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48800952b0413791e1a5c8543532e00d" ns2:_="" ns3:_="">
     <xsd:import namespace="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
@@ -2442,25 +2651,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0257D61C-6042-483B-9C34-3DE0D82CB154}">
   <ds:schemaRefs>
@@ -2470,6 +2660,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
+    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0F2F57-CFBB-4DE2-9688-0C0C6A435162}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2486,15 +2687,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
-    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
excel sheet that helps with which columns to keep and which to remove in order to help create an OLAP database for Power BI
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F833DE9-886A-4AEF-903D-981C8A99B556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569F70DA-7930-42F1-A174-F5FC2AA32E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
@@ -708,8 +708,8 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B75" sqref="A75:XFD75"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2392,25 +2392,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA5D0A6329BB324E86983B32928CFC2E" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b28f3bc5995c0091f528145aa367664">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xmlns:ns3="ced60a7f-99b1-48d2-b555-34851c8026ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48800952b0413791e1a5c8543532e00d" ns2:_="" ns3:_="">
     <xsd:import namespace="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
@@ -2651,6 +2632,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0257D61C-6042-483B-9C34-3DE0D82CB154}">
   <ds:schemaRefs>
@@ -2660,17 +2660,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
-    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0F2F57-CFBB-4DE2-9688-0C0C6A435162}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2687,4 +2676,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
+    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding power bi files with calculated columns and data cleaning and also excel file that helped with data cleaning
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569F70DA-7930-42F1-A174-F5FC2AA32E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{767DC16D-BBDF-45AC-9DEE-DC38706951C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
+    <workbookView xWindow="5304" yWindow="3720" windowWidth="17280" windowHeight="9960" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Northwind Columns" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="96">
   <si>
     <t>table_name</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>varchar</t>
+  </si>
+  <si>
+    <t>remove?</t>
   </si>
 </sst>
 </file>
@@ -707,9 +710,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B56A5E-AA28-4DB9-BAE3-51DE131C631E}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,7 +821,7 @@
         <v>91</v>
       </c>
       <c r="K3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -2392,6 +2395,25 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA5D0A6329BB324E86983B32928CFC2E" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b28f3bc5995c0091f528145aa367664">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xmlns:ns3="ced60a7f-99b1-48d2-b555-34851c8026ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48800952b0413791e1a5c8543532e00d" ns2:_="" ns3:_="">
     <xsd:import namespace="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
@@ -2632,25 +2654,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0257D61C-6042-483B-9C34-3DE0D82CB154}">
   <ds:schemaRefs>
@@ -2660,6 +2663,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
+    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0F2F57-CFBB-4DE2-9688-0C0C6A435162}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2676,15 +2690,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
-    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
created visual after deleting one category table and putting one column of category in product then making hierarchy and crating visual
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{767DC16D-BBDF-45AC-9DEE-DC38706951C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362394DB-72BC-4257-A565-805C4D1F22A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5304" yWindow="3720" windowWidth="17280" windowHeight="9960" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
@@ -283,21 +283,12 @@
     <t>TerritoryDescription</t>
   </si>
   <si>
-    <t>Primary Key?</t>
-  </si>
-  <si>
     <t>Foreign Key?</t>
   </si>
   <si>
     <t>Keep it?</t>
   </si>
   <si>
-    <t>Measure Candidate?</t>
-  </si>
-  <si>
-    <t>Attribute Candidate?</t>
-  </si>
-  <si>
     <t>Formatting Considerations?</t>
   </si>
   <si>
@@ -323,6 +314,15 @@
   </si>
   <si>
     <t>remove?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measure Candidate? Count - min -max </t>
+  </si>
+  <si>
+    <t>Attribute Candidate? Catergorical- as labels in a chart, look up table, dimension table, more sttribute than mesaures</t>
+  </si>
+  <si>
+    <t>Primary Key? For relationship, usually not use in report but their may be instances where you will use in report where you have a natural key</t>
   </si>
 </sst>
 </file>
@@ -710,9 +710,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B56A5E-AA28-4DB9-BAE3-51DE131C631E}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,11 +722,11 @@
     <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="6" max="6" width="116.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.88671875" customWidth="1"/>
     <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="71" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5546875" customWidth="1"/>
   </cols>
@@ -748,31 +748,31 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -792,13 +792,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -818,10 +818,10 @@
         <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -841,7 +841,7 @@
         <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -861,7 +861,7 @@
         <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -881,10 +881,10 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -904,10 +904,10 @@
         <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -927,7 +927,7 @@
         <v>60</v>
       </c>
       <c r="L8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -947,7 +947,7 @@
         <v>60</v>
       </c>
       <c r="L9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -984,7 +984,7 @@
         <v>30</v>
       </c>
       <c r="K11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1055,7 +1055,7 @@
         <v>48</v>
       </c>
       <c r="K15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1075,7 +1075,7 @@
         <v>48</v>
       </c>
       <c r="K16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1095,10 +1095,10 @@
         <v>4</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1220,7 +1220,7 @@
         <v>120</v>
       </c>
       <c r="K24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1308,7 +1308,7 @@
         <v>48</v>
       </c>
       <c r="K29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1328,7 +1328,7 @@
         <v>8</v>
       </c>
       <c r="K30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1348,7 +1348,7 @@
         <v>16</v>
       </c>
       <c r="K31" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1368,7 +1368,7 @@
         <v>16</v>
       </c>
       <c r="K32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1405,7 +1405,7 @@
         <v>510</v>
       </c>
       <c r="K34" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1425,10 +1425,10 @@
         <v>4</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1448,10 +1448,10 @@
         <v>40</v>
       </c>
       <c r="G36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1471,10 +1471,10 @@
         <v>4</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1562,10 +1562,10 @@
         <v>4</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -1585,10 +1585,10 @@
         <v>10</v>
       </c>
       <c r="G43" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -1608,10 +1608,10 @@
         <v>4</v>
       </c>
       <c r="G44" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -1631,7 +1631,7 @@
         <v>8</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -1668,7 +1668,7 @@
         <v>8</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -1722,7 +1722,7 @@
         <v>80</v>
       </c>
       <c r="I50" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -1827,10 +1827,10 @@
         <v>4</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -1850,7 +1850,7 @@
         <v>80</v>
       </c>
       <c r="I57" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -1870,10 +1870,10 @@
         <v>4</v>
       </c>
       <c r="G58" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -1893,10 +1893,10 @@
         <v>4</v>
       </c>
       <c r="G59" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -2018,10 +2018,10 @@
         <v>4</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
@@ -2109,10 +2109,10 @@
         <v>4</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
@@ -2132,7 +2132,7 @@
         <v>80</v>
       </c>
       <c r="I72" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
@@ -2186,7 +2186,7 @@
         <v>120</v>
       </c>
       <c r="K75" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
@@ -2274,7 +2274,7 @@
         <v>48</v>
       </c>
       <c r="K80" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
@@ -2294,7 +2294,7 @@
         <v>48</v>
       </c>
       <c r="K81" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
@@ -2331,10 +2331,10 @@
         <v>40</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
@@ -2371,13 +2371,13 @@
         <v>4</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K85" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2395,25 +2395,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA5D0A6329BB324E86983B32928CFC2E" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b28f3bc5995c0091f528145aa367664">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xmlns:ns3="ced60a7f-99b1-48d2-b555-34851c8026ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48800952b0413791e1a5c8543532e00d" ns2:_="" ns3:_="">
     <xsd:import namespace="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
@@ -2654,6 +2635,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0257D61C-6042-483B-9C34-3DE0D82CB154}">
   <ds:schemaRefs>
@@ -2663,17 +2663,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
-    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0F2F57-CFBB-4DE2-9688-0C0C6A435162}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2690,4 +2679,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
+    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>